<commit_message>
Add Instagram login page
</commit_message>
<xml_diff>
--- a/credentials.xlsx
+++ b/credentials.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Username</t>
   </si>
@@ -25,7 +25,13 @@
     <t>vishal7singh03</t>
   </si>
   <si>
+    <t>r2442tt</t>
+  </si>
+  <si>
     <t>wefggew</t>
+  </si>
+  <si>
+    <t>ggg42g2</t>
   </si>
 </sst>
 </file>
@@ -383,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -402,7 +408,23 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
         <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>